<commit_message>
B2C and B2B Checkout Suites
</commit_message>
<xml_diff>
--- a/resources/testData/MJ_B2B_Login.xlsx
+++ b/resources/testData/MJ_B2B_Login.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="526" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -67,18 +67,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>navedahmed@pragiti.com</t>
-  </si>
-  <si>
     <t>inputUserId</t>
   </si>
   <si>
     <t>inputPassword</t>
   </si>
   <si>
-    <t>checkbox1</t>
-  </si>
-  <si>
     <t>validateUserButton</t>
   </si>
   <si>
@@ -89,16 +83,27 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>navedsmart@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -121,13 +126,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -144,8 +152,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:F6" totalsRowShown="0">
+  <autoFilter ref="A1:F6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TestCaseId"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Action"/>
@@ -162,7 +170,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="UserName"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="UserName" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Password"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -432,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,10 +484,10 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -493,13 +501,13 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -513,18 +521,18 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -533,41 +541,24 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>3000</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>3000</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -584,7 +575,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,17 +604,21 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
+      <c r="A2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B2">
         <v>1234</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{75FA4F1E-B594-42DC-8090-ABD06AA687AE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>